<commit_message>
중간 커밋 ERP > MES
</commit_message>
<xml_diff>
--- a/문서파일보관용/최종문서용/GanttChart/ERPTPGANTTChart.xlsx
+++ b/문서파일보관용/최종문서용/GanttChart/ERPTPGANTTChart.xlsx
@@ -234,10 +234,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ERP 공부</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>버퍼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -262,7 +258,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ERP Team Project</t>
+    <t>MES Team Project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MES 공부</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -733,6 +733,51 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -747,51 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="5" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="4" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,7 +1105,7 @@
   <dimension ref="A2:AI31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1118,91 +1118,91 @@
   <sheetData>
     <row r="2" spans="1:35" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="37" t="s">
+      <c r="B2" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
     </row>
     <row r="3" spans="1:35" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="38" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="38" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="39"/>
-      <c r="AE3" s="39"/>
-      <c r="AF3" s="39"/>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="40"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="41"/>
+      <c r="U3" s="41"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="41"/>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="41"/>
+      <c r="AA3" s="41"/>
+      <c r="AB3" s="41"/>
+      <c r="AC3" s="41"/>
+      <c r="AD3" s="41"/>
+      <c r="AE3" s="41"/>
+      <c r="AF3" s="41"/>
+      <c r="AG3" s="41"/>
+      <c r="AH3" s="41"/>
+      <c r="AI3" s="42"/>
     </row>
     <row r="4" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="24" t="s">
         <v>1</v>
       </c>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="5" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="25"/>
@@ -1307,43 +1307,43 @@
         <v>34</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="46"/>
-      <c r="Z5" s="46"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-      <c r="AC5" s="46"/>
-      <c r="AD5" s="46"/>
-      <c r="AE5" s="46"/>
-      <c r="AF5" s="46"/>
-      <c r="AG5" s="46"/>
-      <c r="AH5" s="46"/>
-      <c r="AI5" s="47"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+      <c r="Z5" s="33"/>
+      <c r="AA5" s="33"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="33"/>
+      <c r="AE5" s="33"/>
+      <c r="AF5" s="33"/>
+      <c r="AG5" s="33"/>
+      <c r="AH5" s="33"/>
+      <c r="AI5" s="34"/>
     </row>
     <row r="6" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="34"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="26"/>
       <c r="D6" s="24" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
@@ -1351,160 +1351,160 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
-      <c r="N6" s="41"/>
-      <c r="O6" s="41"/>
-      <c r="P6" s="41"/>
-      <c r="Q6" s="41"/>
-      <c r="R6" s="41"/>
-      <c r="S6" s="41"/>
-      <c r="T6" s="41"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
-      <c r="Y6" s="41"/>
-      <c r="Z6" s="41"/>
-      <c r="AA6" s="41"/>
-      <c r="AB6" s="41"/>
-      <c r="AC6" s="41"/>
-      <c r="AD6" s="41"/>
-      <c r="AE6" s="41"/>
-      <c r="AF6" s="41"/>
-      <c r="AG6" s="41"/>
-      <c r="AH6" s="41"/>
-      <c r="AI6" s="45"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="32"/>
     </row>
     <row r="7" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
-      <c r="B7" s="35"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="27"/>
       <c r="D7" s="24" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="6"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
-      <c r="N7" s="41"/>
-      <c r="O7" s="41"/>
-      <c r="P7" s="41"/>
-      <c r="Q7" s="41"/>
-      <c r="R7" s="41"/>
-      <c r="S7" s="41"/>
-      <c r="T7" s="41"/>
-      <c r="U7" s="41"/>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41"/>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41"/>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="41"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="41"/>
-      <c r="AG7" s="41"/>
-      <c r="AH7" s="41"/>
-      <c r="AI7" s="45"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
+      <c r="Y7" s="28"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="28"/>
+      <c r="AB7" s="28"/>
+      <c r="AC7" s="28"/>
+      <c r="AD7" s="28"/>
+      <c r="AE7" s="28"/>
+      <c r="AF7" s="28"/>
+      <c r="AG7" s="28"/>
+      <c r="AH7" s="28"/>
+      <c r="AI7" s="32"/>
     </row>
     <row r="8" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="38" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="25"/>
       <c r="D8" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="42"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="41"/>
-      <c r="R8" s="41"/>
-      <c r="S8" s="41"/>
-      <c r="T8" s="41"/>
-      <c r="U8" s="41"/>
-      <c r="V8" s="41"/>
-      <c r="W8" s="41"/>
-      <c r="X8" s="41"/>
-      <c r="Y8" s="41"/>
-      <c r="Z8" s="41"/>
-      <c r="AA8" s="41"/>
-      <c r="AB8" s="41"/>
-      <c r="AC8" s="41"/>
-      <c r="AD8" s="41"/>
-      <c r="AE8" s="41"/>
-      <c r="AF8" s="41"/>
-      <c r="AG8" s="41"/>
-      <c r="AH8" s="41"/>
-      <c r="AI8" s="45"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
+      <c r="Y8" s="28"/>
+      <c r="Z8" s="28"/>
+      <c r="AA8" s="28"/>
+      <c r="AB8" s="28"/>
+      <c r="AC8" s="28"/>
+      <c r="AD8" s="28"/>
+      <c r="AE8" s="28"/>
+      <c r="AF8" s="28"/>
+      <c r="AG8" s="28"/>
+      <c r="AH8" s="28"/>
+      <c r="AI8" s="32"/>
     </row>
     <row r="9" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
-      <c r="B9" s="34"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="26"/>
       <c r="D9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="42"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="41"/>
-      <c r="AC9" s="41"/>
-      <c r="AD9" s="41"/>
-      <c r="AE9" s="41"/>
-      <c r="AF9" s="41"/>
-      <c r="AG9" s="41"/>
-      <c r="AH9" s="41"/>
-      <c r="AI9" s="45"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="32"/>
     </row>
     <row r="10" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="34"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="26"/>
       <c r="D10" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -1512,77 +1512,77 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="41"/>
-      <c r="Q10" s="41"/>
-      <c r="R10" s="41"/>
-      <c r="S10" s="41"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="41"/>
-      <c r="V10" s="41"/>
-      <c r="W10" s="41"/>
-      <c r="X10" s="41"/>
-      <c r="Y10" s="41"/>
-      <c r="Z10" s="41"/>
-      <c r="AA10" s="41"/>
-      <c r="AB10" s="41"/>
-      <c r="AC10" s="41"/>
-      <c r="AD10" s="41"/>
-      <c r="AE10" s="41"/>
-      <c r="AF10" s="41"/>
-      <c r="AG10" s="41"/>
-      <c r="AH10" s="41"/>
-      <c r="AI10" s="45"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="28"/>
+      <c r="AB10" s="28"/>
+      <c r="AC10" s="28"/>
+      <c r="AD10" s="28"/>
+      <c r="AE10" s="28"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="28"/>
+      <c r="AH10" s="28"/>
+      <c r="AI10" s="32"/>
     </row>
     <row r="11" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
-      <c r="B11" s="34"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="26"/>
       <c r="D11" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="42"/>
+      <c r="E11" s="29"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
-      <c r="N11" s="41"/>
-      <c r="O11" s="41"/>
-      <c r="P11" s="41"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="41"/>
-      <c r="S11" s="41"/>
-      <c r="T11" s="41"/>
-      <c r="U11" s="41"/>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
-      <c r="Y11" s="41"/>
-      <c r="Z11" s="41"/>
-      <c r="AA11" s="41"/>
-      <c r="AB11" s="41"/>
-      <c r="AC11" s="41"/>
-      <c r="AD11" s="41"/>
-      <c r="AE11" s="41"/>
-      <c r="AF11" s="41"/>
-      <c r="AG11" s="41"/>
-      <c r="AH11" s="41"/>
-      <c r="AI11" s="45"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
+      <c r="AH11" s="28"/>
+      <c r="AI11" s="32"/>
     </row>
     <row r="12" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="35"/>
+      <c r="B12" s="37"/>
       <c r="C12" s="27"/>
       <c r="D12" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="28"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -1590,562 +1590,562 @@
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
-      <c r="AE12" s="41"/>
-      <c r="AF12" s="41"/>
-      <c r="AG12" s="41"/>
-      <c r="AH12" s="41"/>
-      <c r="AI12" s="45"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="28"/>
+      <c r="Z12" s="28"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="28"/>
+      <c r="AC12" s="28"/>
+      <c r="AD12" s="28"/>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="28"/>
+      <c r="AH12" s="28"/>
+      <c r="AI12" s="32"/>
     </row>
     <row r="13" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>56</v>
+      <c r="C13" s="38" t="s">
+        <v>55</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12"/>
       <c r="R13" s="12"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
-      <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
-      <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
-      <c r="AD13" s="41"/>
-      <c r="AE13" s="41"/>
-      <c r="AF13" s="41"/>
-      <c r="AG13" s="41"/>
-      <c r="AH13" s="41"/>
-      <c r="AI13" s="45"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="32"/>
     </row>
     <row r="14" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
-      <c r="S14" s="41"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
-      <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
-      <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
-      <c r="AD14" s="41"/>
-      <c r="AE14" s="41"/>
-      <c r="AF14" s="41"/>
-      <c r="AG14" s="41"/>
-      <c r="AH14" s="41"/>
-      <c r="AI14" s="45"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="28"/>
+      <c r="Z14" s="28"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="28"/>
+      <c r="AC14" s="28"/>
+      <c r="AD14" s="28"/>
+      <c r="AE14" s="28"/>
+      <c r="AF14" s="28"/>
+      <c r="AG14" s="28"/>
+      <c r="AH14" s="28"/>
+      <c r="AI14" s="32"/>
     </row>
     <row r="15" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12"/>
       <c r="R15" s="12"/>
-      <c r="S15" s="41"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
-      <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
-      <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
-      <c r="AD15" s="41"/>
-      <c r="AE15" s="41"/>
-      <c r="AF15" s="41"/>
-      <c r="AG15" s="41"/>
-      <c r="AH15" s="41"/>
-      <c r="AI15" s="45"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="28"/>
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="28"/>
+      <c r="AH15" s="28"/>
+      <c r="AI15" s="32"/>
     </row>
     <row r="16" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12"/>
       <c r="R16" s="12"/>
-      <c r="S16" s="41"/>
-      <c r="T16" s="41"/>
-      <c r="U16" s="41"/>
-      <c r="V16" s="41"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
-      <c r="Y16" s="41"/>
-      <c r="Z16" s="41"/>
-      <c r="AA16" s="41"/>
-      <c r="AB16" s="41"/>
-      <c r="AC16" s="41"/>
-      <c r="AD16" s="41"/>
-      <c r="AE16" s="41"/>
-      <c r="AF16" s="41"/>
-      <c r="AG16" s="41"/>
-      <c r="AH16" s="41"/>
-      <c r="AI16" s="45"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="28"/>
+      <c r="Z16" s="28"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="28"/>
+      <c r="AC16" s="28"/>
+      <c r="AD16" s="28"/>
+      <c r="AE16" s="28"/>
+      <c r="AF16" s="28"/>
+      <c r="AG16" s="28"/>
+      <c r="AH16" s="28"/>
+      <c r="AI16" s="32"/>
     </row>
     <row r="17" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
       <c r="D17" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="41"/>
-      <c r="L17" s="41"/>
-      <c r="M17" s="41"/>
-      <c r="N17" s="41"/>
-      <c r="O17" s="41"/>
-      <c r="P17" s="41"/>
-      <c r="Q17" s="41"/>
-      <c r="R17" s="41"/>
+        <v>54</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
-      <c r="U17" s="41"/>
-      <c r="V17" s="41"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
-      <c r="Y17" s="41"/>
-      <c r="Z17" s="41"/>
-      <c r="AA17" s="41"/>
-      <c r="AB17" s="41"/>
-      <c r="AC17" s="41"/>
-      <c r="AD17" s="41"/>
-      <c r="AE17" s="41"/>
-      <c r="AF17" s="41"/>
-      <c r="AG17" s="41"/>
-      <c r="AH17" s="41"/>
-      <c r="AI17" s="45"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28"/>
+      <c r="AE17" s="28"/>
+      <c r="AF17" s="28"/>
+      <c r="AG17" s="28"/>
+      <c r="AH17" s="28"/>
+      <c r="AI17" s="32"/>
     </row>
     <row r="18" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="33" t="s">
-        <v>57</v>
+      <c r="B18" s="36"/>
+      <c r="C18" s="38" t="s">
+        <v>56</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
       <c r="U18" s="14"/>
       <c r="V18" s="14"/>
       <c r="W18" s="14"/>
       <c r="X18" s="14"/>
       <c r="Y18" s="14"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="41"/>
-      <c r="AC18" s="41"/>
-      <c r="AD18" s="41"/>
-      <c r="AE18" s="41"/>
-      <c r="AF18" s="41"/>
-      <c r="AG18" s="41"/>
-      <c r="AH18" s="41"/>
-      <c r="AI18" s="45"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
+      <c r="AD18" s="28"/>
+      <c r="AE18" s="28"/>
+      <c r="AF18" s="28"/>
+      <c r="AG18" s="28"/>
+      <c r="AH18" s="28"/>
+      <c r="AI18" s="32"/>
     </row>
     <row r="19" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="42"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41"/>
-      <c r="P19" s="41"/>
-      <c r="Q19" s="41"/>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
       <c r="U19" s="14"/>
       <c r="V19" s="14"/>
       <c r="W19" s="14"/>
       <c r="X19" s="14"/>
       <c r="Y19" s="14"/>
-      <c r="Z19" s="41"/>
-      <c r="AA19" s="41"/>
-      <c r="AB19" s="41"/>
-      <c r="AC19" s="41"/>
-      <c r="AD19" s="41"/>
-      <c r="AE19" s="41"/>
-      <c r="AF19" s="41"/>
-      <c r="AG19" s="41"/>
-      <c r="AH19" s="41"/>
-      <c r="AI19" s="45"/>
+      <c r="Z19" s="28"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="28"/>
+      <c r="AC19" s="28"/>
+      <c r="AD19" s="28"/>
+      <c r="AE19" s="28"/>
+      <c r="AF19" s="28"/>
+      <c r="AG19" s="28"/>
+      <c r="AH19" s="28"/>
+      <c r="AI19" s="32"/>
     </row>
     <row r="20" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="42"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="28"/>
       <c r="U20" s="14"/>
       <c r="V20" s="14"/>
       <c r="W20" s="14"/>
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="41"/>
-      <c r="AC20" s="41"/>
-      <c r="AD20" s="41"/>
-      <c r="AE20" s="41"/>
-      <c r="AF20" s="41"/>
-      <c r="AG20" s="41"/>
-      <c r="AH20" s="41"/>
-      <c r="AI20" s="45"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="28"/>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="28"/>
+      <c r="AE20" s="28"/>
+      <c r="AF20" s="28"/>
+      <c r="AG20" s="28"/>
+      <c r="AH20" s="28"/>
+      <c r="AI20" s="32"/>
     </row>
     <row r="21" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41"/>
-      <c r="P21" s="41"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-      <c r="T21" s="41"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
       <c r="U21" s="14"/>
       <c r="V21" s="14"/>
       <c r="W21" s="14"/>
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
-      <c r="Z21" s="41"/>
-      <c r="AA21" s="41"/>
-      <c r="AB21" s="41"/>
-      <c r="AC21" s="41"/>
-      <c r="AD21" s="41"/>
-      <c r="AE21" s="41"/>
-      <c r="AF21" s="41"/>
-      <c r="AG21" s="41"/>
-      <c r="AH21" s="41"/>
-      <c r="AI21" s="45"/>
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="28"/>
+      <c r="AE21" s="28"/>
+      <c r="AF21" s="28"/>
+      <c r="AG21" s="28"/>
+      <c r="AH21" s="28"/>
+      <c r="AI21" s="32"/>
     </row>
     <row r="22" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="33" t="s">
-        <v>58</v>
+      <c r="B22" s="36"/>
+      <c r="C22" s="38" t="s">
+        <v>57</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
-      <c r="U22" s="41"/>
-      <c r="V22" s="41"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
-      <c r="Y22" s="41"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="28"/>
+      <c r="V22" s="28"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="28"/>
+      <c r="Y22" s="28"/>
       <c r="Z22" s="15"/>
       <c r="AA22" s="15"/>
-      <c r="AB22" s="41"/>
-      <c r="AC22" s="41"/>
-      <c r="AD22" s="41"/>
-      <c r="AE22" s="41"/>
-      <c r="AF22" s="41"/>
-      <c r="AG22" s="41"/>
-      <c r="AH22" s="41"/>
-      <c r="AI22" s="45"/>
+      <c r="AB22" s="28"/>
+      <c r="AC22" s="28"/>
+      <c r="AD22" s="28"/>
+      <c r="AE22" s="28"/>
+      <c r="AF22" s="28"/>
+      <c r="AG22" s="28"/>
+      <c r="AH22" s="28"/>
+      <c r="AI22" s="32"/>
     </row>
     <row r="23" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
       <c r="D23" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-      <c r="T23" s="41"/>
-      <c r="U23" s="41"/>
-      <c r="V23" s="41"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="41"/>
-      <c r="Y23" s="41"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="28"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="28"/>
+      <c r="V23" s="28"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="28"/>
       <c r="Z23" s="15"/>
       <c r="AA23" s="15"/>
-      <c r="AB23" s="41"/>
-      <c r="AC23" s="41"/>
-      <c r="AD23" s="41"/>
-      <c r="AE23" s="41"/>
-      <c r="AF23" s="41"/>
-      <c r="AG23" s="41"/>
-      <c r="AH23" s="41"/>
-      <c r="AI23" s="45"/>
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="28"/>
+      <c r="AD23" s="28"/>
+      <c r="AE23" s="28"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="28"/>
+      <c r="AH23" s="28"/>
+      <c r="AI23" s="32"/>
     </row>
     <row r="24" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
       <c r="D24" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
-      <c r="T24" s="41"/>
-      <c r="U24" s="41"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
-      <c r="Y24" s="41"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="28"/>
+      <c r="V24" s="28"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="28"/>
+      <c r="Y24" s="28"/>
       <c r="Z24" s="15"/>
       <c r="AA24" s="15"/>
-      <c r="AB24" s="41"/>
-      <c r="AC24" s="41"/>
-      <c r="AD24" s="41"/>
-      <c r="AE24" s="41"/>
-      <c r="AF24" s="41"/>
-      <c r="AG24" s="41"/>
-      <c r="AH24" s="41"/>
-      <c r="AI24" s="45"/>
+      <c r="AB24" s="28"/>
+      <c r="AC24" s="28"/>
+      <c r="AD24" s="28"/>
+      <c r="AE24" s="28"/>
+      <c r="AF24" s="28"/>
+      <c r="AG24" s="28"/>
+      <c r="AH24" s="28"/>
+      <c r="AI24" s="32"/>
     </row>
     <row r="25" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-      <c r="T25" s="41"/>
-      <c r="U25" s="41"/>
-      <c r="V25" s="41"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
-      <c r="Y25" s="41"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="28"/>
+      <c r="T25" s="28"/>
+      <c r="U25" s="28"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="28"/>
+      <c r="X25" s="28"/>
+      <c r="Y25" s="28"/>
       <c r="Z25" s="15"/>
       <c r="AA25" s="15"/>
-      <c r="AB25" s="41"/>
-      <c r="AC25" s="41"/>
-      <c r="AD25" s="41"/>
-      <c r="AE25" s="41"/>
-      <c r="AF25" s="41"/>
-      <c r="AG25" s="41"/>
-      <c r="AH25" s="41"/>
-      <c r="AI25" s="45"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="28"/>
+      <c r="AE25" s="28"/>
+      <c r="AF25" s="28"/>
+      <c r="AG25" s="28"/>
+      <c r="AH25" s="28"/>
+      <c r="AI25" s="32"/>
     </row>
     <row r="26" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="33" t="s">
-        <v>59</v>
+      <c r="B26" s="36"/>
+      <c r="C26" s="38" t="s">
+        <v>58</v>
       </c>
       <c r="D26" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
       <c r="P26" s="16"/>
@@ -2160,31 +2160,31 @@
       <c r="Y26" s="16"/>
       <c r="Z26" s="16"/>
       <c r="AA26" s="16"/>
-      <c r="AB26" s="41"/>
-      <c r="AC26" s="41"/>
-      <c r="AD26" s="41"/>
-      <c r="AE26" s="41"/>
-      <c r="AF26" s="41"/>
-      <c r="AG26" s="41"/>
-      <c r="AH26" s="41"/>
-      <c r="AI26" s="45"/>
+      <c r="AB26" s="28"/>
+      <c r="AC26" s="28"/>
+      <c r="AD26" s="28"/>
+      <c r="AE26" s="28"/>
+      <c r="AF26" s="28"/>
+      <c r="AG26" s="28"/>
+      <c r="AH26" s="28"/>
+      <c r="AI26" s="32"/>
     </row>
     <row r="27" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
       <c r="D27" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="42"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
       <c r="N27" s="17"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
@@ -2201,85 +2201,85 @@
       <c r="AA27" s="17"/>
       <c r="AB27" s="17"/>
       <c r="AC27" s="17"/>
-      <c r="AD27" s="41"/>
-      <c r="AE27" s="41"/>
-      <c r="AF27" s="41"/>
-      <c r="AG27" s="41"/>
-      <c r="AH27" s="41"/>
-      <c r="AI27" s="45"/>
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="28"/>
+      <c r="AF27" s="28"/>
+      <c r="AG27" s="28"/>
+      <c r="AH27" s="28"/>
+      <c r="AI27" s="32"/>
     </row>
     <row r="28" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>51</v>
       </c>
       <c r="C28" s="25"/>
       <c r="D28" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="42"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41"/>
-      <c r="P28" s="41"/>
-      <c r="Q28" s="41"/>
-      <c r="R28" s="41"/>
-      <c r="S28" s="41"/>
-      <c r="T28" s="41"/>
-      <c r="U28" s="41"/>
-      <c r="V28" s="41"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
-      <c r="Y28" s="41"/>
-      <c r="Z28" s="41"/>
-      <c r="AA28" s="41"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="28"/>
+      <c r="V28" s="28"/>
+      <c r="W28" s="28"/>
+      <c r="X28" s="28"/>
+      <c r="Y28" s="28"/>
+      <c r="Z28" s="28"/>
+      <c r="AA28" s="28"/>
       <c r="AB28" s="18"/>
       <c r="AC28" s="18"/>
       <c r="AD28" s="18"/>
       <c r="AE28" s="18"/>
       <c r="AF28" s="18"/>
       <c r="AG28" s="18"/>
-      <c r="AH28" s="41"/>
-      <c r="AI28" s="45"/>
+      <c r="AH28" s="28"/>
+      <c r="AI28" s="32"/>
     </row>
     <row r="29" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="B29" s="34"/>
+      <c r="B29" s="36"/>
       <c r="C29" s="26"/>
       <c r="D29" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="42"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="41"/>
-      <c r="V29" s="41"/>
-      <c r="W29" s="41"/>
-      <c r="X29" s="41"/>
-      <c r="Y29" s="41"/>
-      <c r="Z29" s="41"/>
-      <c r="AA29" s="41"/>
-      <c r="AB29" s="41"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="28"/>
+      <c r="V29" s="28"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="28"/>
+      <c r="Y29" s="28"/>
+      <c r="Z29" s="28"/>
+      <c r="AA29" s="28"/>
+      <c r="AB29" s="28"/>
       <c r="AC29" s="19"/>
       <c r="AD29" s="19"/>
       <c r="AE29" s="19"/>
@@ -2290,78 +2290,78 @@
     </row>
     <row r="30" spans="1:35" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
-      <c r="B30" s="34"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="26"/>
       <c r="D30" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="42"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
-      <c r="R30" s="41"/>
-      <c r="S30" s="41"/>
-      <c r="T30" s="41"/>
-      <c r="U30" s="41"/>
-      <c r="V30" s="41"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="41"/>
-      <c r="Y30" s="41"/>
-      <c r="Z30" s="41"/>
-      <c r="AA30" s="41"/>
-      <c r="AB30" s="41"/>
-      <c r="AC30" s="41"/>
-      <c r="AD30" s="41"/>
-      <c r="AE30" s="41"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="28"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="28"/>
+      <c r="X30" s="28"/>
+      <c r="Y30" s="28"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="28"/>
+      <c r="AC30" s="28"/>
+      <c r="AD30" s="28"/>
+      <c r="AE30" s="28"/>
       <c r="AF30" s="21"/>
       <c r="AG30" s="21"/>
       <c r="AH30" s="21"/>
-      <c r="AI30" s="45"/>
+      <c r="AI30" s="32"/>
     </row>
     <row r="31" spans="1:35" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
-      <c r="B31" s="35"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="27"/>
       <c r="D31" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="43"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
-      <c r="S31" s="44"/>
-      <c r="T31" s="44"/>
-      <c r="U31" s="44"/>
-      <c r="V31" s="44"/>
-      <c r="W31" s="44"/>
-      <c r="X31" s="44"/>
-      <c r="Y31" s="44"/>
-      <c r="Z31" s="44"/>
-      <c r="AA31" s="44"/>
-      <c r="AB31" s="44"/>
-      <c r="AC31" s="44"/>
-      <c r="AD31" s="44"/>
-      <c r="AE31" s="44"/>
-      <c r="AF31" s="44"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="31"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="31"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="31"/>
+      <c r="X31" s="31"/>
+      <c r="Y31" s="31"/>
+      <c r="Z31" s="31"/>
+      <c r="AA31" s="31"/>
+      <c r="AB31" s="31"/>
+      <c r="AC31" s="31"/>
+      <c r="AD31" s="31"/>
+      <c r="AE31" s="31"/>
+      <c r="AF31" s="31"/>
       <c r="AG31" s="22"/>
       <c r="AH31" s="22"/>
       <c r="AI31" s="23"/>

</xml_diff>